<commit_message>
Commiting test case NewProduct
</commit_message>
<xml_diff>
--- a/WordpressDemo/data/login.xlsx
+++ b/WordpressDemo/data/login.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11890" windowHeight="4120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11890" windowHeight="3760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>UserName</t>
   </si>
@@ -44,6 +44,24 @@
   </si>
   <si>
     <t>abc123</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Sale Price</t>
+  </si>
+  <si>
+    <t>Itemnumber</t>
+  </si>
+  <si>
+    <t>Ac10</t>
+  </si>
+  <si>
+    <t>Butter</t>
   </si>
 </sst>
 </file>
@@ -88,11 +106,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -398,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -411,10 +430,13 @@
     <col min="3" max="3" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="6" max="7" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,8 +452,20 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -446,6 +480,18 @@
       </c>
       <c r="E2" s="3">
         <v>1000</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>